<commit_message>
Saving collection, updating steel scrap treatment, splitting grades
Saving old scrap collection in results, updating steel scrap treatment from being direct melt only to refining only, splitting grades to have operating mines and incentive mines ore grades change at different rates.
Unsure what happened that caused scenario setup to get updated
</commit_message>
<xml_diff>
--- a/Scenario setup.xlsx
+++ b/Scenario setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA4F623-7E55-4E4E-B60D-29B00316CE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FB41A2-1C76-CD45-824A-3DD389493AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{19F7A473-1970-354B-A27C-175479056876}"/>
   </bookViews>
@@ -1348,7 +1348,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L54" sqref="L54"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Clarifying edit as to how to use Scenario setup.xlsx
</commit_message>
<xml_diff>
--- a/Scenario setup.xlsx
+++ b/Scenario setup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C8CFB7-9D76-664A-8FE5-AC98EFFDB9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14208FD8-D81D-2648-B735-D493DB1C55D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="1" xr2:uid="{19F7A473-1970-354B-A27C-175479056876}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="307">
   <si>
     <t>Parameter category</t>
   </si>
@@ -954,6 +954,9 @@
   </si>
   <si>
     <t>Basic operation:</t>
+  </si>
+  <si>
+    <t>Run the model using these values by calling the Many.run_future_scenarios function with the scenario_sheet_file_path variable as a string pointing to this file.</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1078,29 +1081,14 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1142,6 +1130,24 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1156,14 +1162,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}" name="Table1" displayName="Table1" ref="A1:M99" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}" name="Table1" displayName="Table1" ref="A1:M99" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:M99" xr:uid="{3BBC0018-B41E-174D-8CAB-6619D3E5A42C}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{C4332FCF-8E4C-4F49-8EFC-804C6E3A59B2}" name="Parameter category"/>
-    <tableColumn id="2" xr3:uid="{A55A75DB-88A1-1245-BF1A-68A78F78C819}" name="Parameter name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{A55A75DB-88A1-1245-BF1A-68A78F78C819}" name="Parameter name" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{5A41921B-736C-6B44-9ECB-CB018A2EAD98}" name="Variable name"/>
-    <tableColumn id="4" xr3:uid="{AC20CA22-09A0-874C-8AAB-D90343AC4C41}" name="Description" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{BC697E1E-B29C-C449-B77E-41BE3FCCCC5F}" name="Tuning range or preset value" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{AC20CA22-09A0-874C-8AAB-D90343AC4C41}" name="Description" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{BC697E1E-B29C-C449-B77E-41BE3FCCCC5F}" name="Tuning range or preset value" dataDxfId="0"/>
     <tableColumn id="6" xr3:uid="{5E98ED95-4E7B-3B45-A47B-AF1FEE1A9A80}" name="Scenario 1"/>
     <tableColumn id="7" xr3:uid="{D0B2B3FA-F3D8-C746-B783-084B2C487DBB}" name="Scenario 2"/>
     <tableColumn id="8" xr3:uid="{BB62F53F-FC7E-0241-8EFE-9D0D4B695FC4}" name="Scenario 3"/>
@@ -3197,10 +3203,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD35743A-9BCD-4440-A2B9-C15CACDD5C34}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3216,27 +3222,14 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="44" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+    <row r="2" spans="1:14" ht="44" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="3" spans="1:14" ht="44" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>270</v>
+        <v>294</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -3252,9 +3245,9 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
     </row>
-    <row r="4" spans="1:14" ht="22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="44" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -3270,9 +3263,9 @@
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:14" ht="44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="22" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -3290,7 +3283,7 @@
     </row>
     <row r="6" spans="1:14" ht="44" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="14"/>
@@ -3308,7 +3301,7 @@
     </row>
     <row r="7" spans="1:14" ht="44" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -3324,9 +3317,9 @@
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
     </row>
-    <row r="8" spans="1:14" ht="110" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="44" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="14"/>
@@ -3342,8 +3335,10 @@
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
     </row>
-    <row r="9" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:14" ht="110" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>290</v>
+      </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -3358,10 +3353,8 @@
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
     </row>
-    <row r="10" spans="1:14" ht="22" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>299</v>
-      </c>
+    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -3376,9 +3369,9 @@
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
     </row>
-    <row r="11" spans="1:14" ht="132" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>298</v>
+    <row r="11" spans="1:14" ht="22" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>299</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -3394,9 +3387,9 @@
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
     </row>
-    <row r="12" spans="1:14" ht="88" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="132" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -3412,9 +3405,9 @@
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
     </row>
-    <row r="13" spans="1:14" ht="110" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="88" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -3430,9 +3423,9 @@
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
     </row>
-    <row r="14" spans="1:14" ht="132" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="110" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -3448,8 +3441,10 @@
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
     </row>
-    <row r="15" spans="1:14" ht="21" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+    <row r="15" spans="1:14" ht="132" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>303</v>
+      </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -3464,10 +3459,8 @@
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
     </row>
-    <row r="16" spans="1:14" ht="22" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>302</v>
-      </c>
+    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.2">
+      <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -3482,9 +3475,9 @@
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
     </row>
-    <row r="17" spans="1:14" ht="66" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>304</v>
+    <row r="17" spans="1:14" ht="22" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>302</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -3500,8 +3493,10 @@
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
     </row>
-    <row r="18" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+    <row r="18" spans="1:14" ht="66" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>304</v>
+      </c>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -3628,6 +3623,22 @@
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
     </row>
+    <row r="26" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>